<commit_message>
IEEEST supports remote bus specified by `busr`
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_pss.xlsx
+++ b/andes/cases/kundur/kundur_pss.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuiha\andes_github\andes\cases\kundur\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89EB89B4-1EC8-4A7B-850A-F3F4EB22743F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="19140" yWindow="5040" windowWidth="23160" windowHeight="15435" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="25980" windowHeight="14025" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -22,15 +16,18 @@
     <sheet name="GENROU" sheetId="7" r:id="rId7"/>
     <sheet name="TGOV1" sheetId="8" r:id="rId8"/>
     <sheet name="EXDC2" sheetId="9" r:id="rId9"/>
-    <sheet name="Toggler" sheetId="10" r:id="rId10"/>
-    <sheet name="IEEEST" sheetId="11" r:id="rId11"/>
+    <sheet name="IEEEST" sheetId="10" r:id="rId10"/>
+    <sheet name="Toggler" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="136">
+  <si>
+    <t>uid</t>
+  </si>
   <si>
     <t>idx</t>
   </si>
@@ -71,9 +68,6 @@
     <t>owner</t>
   </si>
   <si>
-    <t>uid</t>
-  </si>
-  <si>
     <t>bus</t>
   </si>
   <si>
@@ -374,6 +368,57 @@
     <t>EXDC2_4</t>
   </si>
   <si>
+    <t>avr</t>
+  </si>
+  <si>
+    <t>MODE</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>LSMAX</t>
+  </si>
+  <si>
+    <t>LSMIN</t>
+  </si>
+  <si>
+    <t>VCU</t>
+  </si>
+  <si>
+    <t>VCL</t>
+  </si>
+  <si>
+    <t>IEEEST_1</t>
+  </si>
+  <si>
     <t>model</t>
   </si>
   <si>
@@ -387,69 +432,24 @@
   </si>
   <si>
     <t>Line</t>
-  </si>
-  <si>
-    <t>avr</t>
-  </si>
-  <si>
-    <t>MODE</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>T4</t>
-  </si>
-  <si>
-    <t>T5</t>
-  </si>
-  <si>
-    <t>T6</t>
-  </si>
-  <si>
-    <t>KS</t>
-  </si>
-  <si>
-    <t>LSMAX</t>
-  </si>
-  <si>
-    <t>LSMIN</t>
-  </si>
-  <si>
-    <t>VCU</t>
-  </si>
-  <si>
-    <t>VCL</t>
-  </si>
-  <si>
-    <t>IEEEST_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -457,19 +457,356 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -492,9 +829,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -502,17 +1081,61 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -561,7 +1184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,27 +1216,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -645,24 +1250,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -833,66 +1420,67 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -909,7 +1497,7 @@
         <v>20</v>
       </c>
       <c r="F2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G2">
         <v>0.9</v>
@@ -918,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0.57025491716260168</v>
+        <v>0.570254917162602</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -936,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -953,7 +1541,7 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G3">
         <v>0.9</v>
@@ -962,7 +1550,7 @@
         <v>0.99761</v>
       </c>
       <c r="I3">
-        <v>0.36874618304434781</v>
+        <v>0.368746183044348</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -980,7 +1568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -997,16 +1585,16 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G4">
         <v>0.9</v>
       </c>
       <c r="H4">
-        <v>0.96262999999999999</v>
+        <v>0.96263</v>
       </c>
       <c r="I4">
-        <v>0.18531731464750281</v>
+        <v>0.185317314647503</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1024,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1041,16 +1629,16 @@
         <v>20</v>
       </c>
       <c r="F5">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G5">
         <v>0.9</v>
       </c>
       <c r="H5">
-        <v>0.81691000000000003</v>
+        <v>0.81691</v>
       </c>
       <c r="I5">
-        <v>0.46235866280431398</v>
+        <v>0.462358662804314</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1068,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1085,16 +1673,16 @@
         <v>230</v>
       </c>
       <c r="F6">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G6">
         <v>0.9</v>
       </c>
       <c r="H6">
-        <v>0.97928000000000004</v>
+        <v>0.97928</v>
       </c>
       <c r="I6">
-        <v>0.48020290907670382</v>
+        <v>0.480202909076704</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1112,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1129,16 +1717,16 @@
         <v>230</v>
       </c>
       <c r="F7">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G7">
         <v>0.9</v>
       </c>
       <c r="H7">
-        <v>0.95796000000000003</v>
+        <v>0.95796</v>
       </c>
       <c r="I7">
-        <v>0.28388652948313292</v>
+        <v>0.283886529483133</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1156,7 +1744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1173,16 +1761,16 @@
         <v>230</v>
       </c>
       <c r="F8">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G8">
         <v>0.9</v>
       </c>
       <c r="H8">
-        <v>0.93620000000000003</v>
+        <v>0.9362</v>
       </c>
       <c r="I8">
-        <v>0.12690114458325361</v>
+        <v>0.126901144583254</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1200,7 +1788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1217,16 +1805,16 @@
         <v>230</v>
       </c>
       <c r="F9">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G9">
         <v>0.9</v>
       </c>
       <c r="H9">
-        <v>0.87904000000000004</v>
+        <v>0.87904</v>
       </c>
       <c r="I9">
-        <v>-8.0592323540088801E-2</v>
+        <v>-0.0805923235400888</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1244,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1261,7 +1849,7 @@
         <v>230</v>
       </c>
       <c r="F10">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G10">
         <v>0.9</v>
@@ -1270,7 +1858,7 @@
         <v>0.89054</v>
       </c>
       <c r="I10">
-        <v>9.3617715747722263E-2</v>
+        <v>0.0936177157477223</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1288,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1305,16 +1893,16 @@
         <v>230</v>
       </c>
       <c r="F11">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G11">
         <v>0.9</v>
       </c>
       <c r="H11">
-        <v>0.82957999999999998</v>
+        <v>0.82958</v>
       </c>
       <c r="I11">
-        <v>0.33660070888111671</v>
+        <v>0.336600708881117</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1334,44 +1922,214 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>0.3</v>
+      </c>
+      <c r="V2">
+        <v>-0.3</v>
+      </c>
+      <c r="W2">
+        <v>1.2</v>
+      </c>
+      <c r="X2">
+        <v>0.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="6"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1382,10 +2140,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="F2" t="s">
         <v>51</v>
@@ -1396,193 +2154,41 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:W2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W3" sqref="W3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>0.3</v>
-      </c>
-      <c r="U2">
-        <v>-0.3</v>
-      </c>
-      <c r="V2">
-        <v>1.2</v>
-      </c>
-      <c r="W2">
-        <v>0.8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>15</v>
@@ -1591,16 +2197,16 @@
         <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1620,10 +2226,10 @@
         <v>11.59</v>
       </c>
       <c r="H2">
-        <v>-0.73499999999999999</v>
+        <v>-0.735</v>
       </c>
       <c r="I2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J2">
         <v>0.9</v>
@@ -1632,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1652,10 +2258,10 @@
         <v>15.75</v>
       </c>
       <c r="H3">
-        <v>-0.89900000000000002</v>
+        <v>-0.899</v>
       </c>
       <c r="I3">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J3">
         <v>0.9</v>
@@ -1666,38 +2272,41 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -1724,13 +2333,13 @@
         <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>25</v>
@@ -1739,7 +2348,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1792,7 +2401,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1845,7 +2454,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1900,38 +2509,41 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -1958,13 +2570,13 @@
         <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>25</v>
@@ -1973,10 +2585,10 @@
         <v>26</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1996,10 +2608,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>7.4586100000000002</v>
+        <v>7.45861</v>
       </c>
       <c r="J2">
-        <v>1.4361200000000001</v>
+        <v>1.43612</v>
       </c>
       <c r="K2">
         <v>9</v>
@@ -2029,37 +2641,40 @@
         <v>0.25</v>
       </c>
       <c r="T2">
-        <v>0.57025491716260168</v>
+        <v>0.570254917162602</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>27</v>
@@ -2113,16 +2728,16 @@
         <v>42</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2151,13 +2766,13 @@
         <v>230</v>
       </c>
       <c r="K2">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="L2">
         <v>0.05</v>
       </c>
       <c r="M2">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -2184,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2213,13 +2828,13 @@
         <v>230</v>
       </c>
       <c r="K3">
-        <v>5.0099999999999997E-3</v>
+        <v>0.00501</v>
       </c>
       <c r="L3">
-        <v>5.0009999999999999E-2</v>
+        <v>0.05001</v>
       </c>
       <c r="M3">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -2246,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2275,7 +2890,7 @@
         <v>230</v>
       </c>
       <c r="K4">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="L4">
         <v>0.02</v>
@@ -2308,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2337,10 +2952,10 @@
         <v>230</v>
       </c>
       <c r="K5">
-        <v>2.0100000000000001E-3</v>
+        <v>0.00201</v>
       </c>
       <c r="L5">
-        <v>2.001E-2</v>
+        <v>0.02001</v>
       </c>
       <c r="M5">
         <v>0.03</v>
@@ -2370,7 +2985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2399,10 +3014,10 @@
         <v>230</v>
       </c>
       <c r="K6">
-        <v>2.2009999999999998E-2</v>
+        <v>0.02201</v>
       </c>
       <c r="L6">
-        <v>0.22001000000000001</v>
+        <v>0.22001</v>
       </c>
       <c r="M6">
         <v>0.33</v>
@@ -2432,7 +3047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2461,10 +3076,10 @@
         <v>230</v>
       </c>
       <c r="K7">
-        <v>2.2020000000000001E-2</v>
+        <v>0.02202</v>
       </c>
       <c r="L7">
-        <v>0.22001999999999999</v>
+        <v>0.22002</v>
       </c>
       <c r="M7">
         <v>0.33</v>
@@ -2494,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2523,7 +3138,7 @@
         <v>230</v>
       </c>
       <c r="K8">
-        <v>2.1999999999999999E-2</v>
+        <v>0.022</v>
       </c>
       <c r="L8">
         <v>0.22</v>
@@ -2556,7 +3171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2585,7 +3200,7 @@
         <v>230</v>
       </c>
       <c r="K9">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="L9">
         <v>0.02</v>
@@ -2618,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2647,10 +3262,10 @@
         <v>230</v>
       </c>
       <c r="K10">
-        <v>2.0100000000000001E-3</v>
+        <v>0.00201</v>
       </c>
       <c r="L10">
-        <v>2.001E-2</v>
+        <v>0.02001</v>
       </c>
       <c r="M10">
         <v>0.03</v>
@@ -2680,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2709,13 +3324,13 @@
         <v>230</v>
       </c>
       <c r="K11">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="L11">
         <v>0.05</v>
       </c>
       <c r="M11">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -2742,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2771,13 +3386,13 @@
         <v>230</v>
       </c>
       <c r="K12">
-        <v>5.0099999999999997E-3</v>
+        <v>0.00501</v>
       </c>
       <c r="L12">
-        <v>5.0009999999999999E-2</v>
+        <v>0.05001</v>
       </c>
       <c r="M12">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -2804,7 +3419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2833,10 +3448,10 @@
         <v>230</v>
       </c>
       <c r="K13">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L13">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2866,7 +3481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2895,10 +3510,10 @@
         <v>230</v>
       </c>
       <c r="K14">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L14">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -2928,7 +3543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2957,10 +3572,10 @@
         <v>230</v>
       </c>
       <c r="K15">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L15">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -2990,7 +3605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3019,10 +3634,10 @@
         <v>230</v>
       </c>
       <c r="K16">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L16">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -3054,35 +3669,38 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3096,7 +3714,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3112,32 +3730,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -3152,7 +3773,7 @@
         <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>29</v>
@@ -3212,7 +3833,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3277,7 +3898,7 @@
         <v>0.25</v>
       </c>
       <c r="W2">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X2">
         <v>0.25</v>
@@ -3295,7 +3916,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3360,7 +3981,7 @@
         <v>0.25</v>
       </c>
       <c r="W3">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X3">
         <v>0.25</v>
@@ -3378,7 +3999,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3443,7 +4064,7 @@
         <v>0.25</v>
       </c>
       <c r="W4">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X4">
         <v>0.25</v>
@@ -3461,7 +4082,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3526,7 +4147,7 @@
         <v>0.25</v>
       </c>
       <c r="W5">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X5">
         <v>0.25</v>
@@ -3546,32 +4167,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>83</v>
@@ -3601,7 +4225,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3642,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3683,7 +4307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3724,7 +4348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3767,32 +4391,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>83</v>
@@ -3849,7 +4476,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3884,7 +4511,7 @@
         <v>1.246</v>
       </c>
       <c r="L2">
-        <v>7.5399999999999995E-2</v>
+        <v>0.0754</v>
       </c>
       <c r="M2">
         <v>20</v>
@@ -3917,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3952,7 +4579,7 @@
         <v>1.246</v>
       </c>
       <c r="L3">
-        <v>7.5399999999999995E-2</v>
+        <v>0.0754</v>
       </c>
       <c r="M3">
         <v>20</v>
@@ -3985,7 +4612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4020,7 +4647,7 @@
         <v>1.246</v>
       </c>
       <c r="L4">
-        <v>7.5399999999999995E-2</v>
+        <v>0.0754</v>
       </c>
       <c r="M4">
         <v>20</v>
@@ -4053,7 +4680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4088,7 +4715,7 @@
         <v>1.246</v>
       </c>
       <c r="L5">
-        <v>7.5399999999999995E-2</v>
+        <v>0.0754</v>
       </c>
       <c r="M5">
         <v>20</v>
@@ -4123,5 +4750,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Restored kundur_pss.xlsx to mode 1; Fixed chattering issue in Derivative; Added repr for Delay
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_pss.xlsx
+++ b/andes/cases/kundur/kundur_pss.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56877F4-88A1-3742-92C1-4FB50A1C538E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="25980" windowHeight="14025" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30040" windowHeight="24340" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -437,14 +443,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,353 +460,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -829,251 +492,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1081,61 +502,17 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1420,23 +797,22 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1497,7 +873,7 @@
         <v>20</v>
       </c>
       <c r="F2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G2">
         <v>0.9</v>
@@ -1506,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0.570254917162602</v>
+        <v>0.57025491716260202</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -1524,7 +900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1541,7 +917,7 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G3">
         <v>0.9</v>
@@ -1550,7 +926,7 @@
         <v>0.99761</v>
       </c>
       <c r="I3">
-        <v>0.368746183044348</v>
+        <v>0.36874618304434797</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1568,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1585,16 +961,16 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G4">
         <v>0.9</v>
       </c>
       <c r="H4">
-        <v>0.96263</v>
+        <v>0.96262999999999999</v>
       </c>
       <c r="I4">
-        <v>0.185317314647503</v>
+        <v>0.18531731464750301</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1612,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1629,16 +1005,16 @@
         <v>20</v>
       </c>
       <c r="F5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G5">
         <v>0.9</v>
       </c>
       <c r="H5">
-        <v>0.81691</v>
+        <v>0.81691000000000003</v>
       </c>
       <c r="I5">
-        <v>0.462358662804314</v>
+        <v>0.46235866280431398</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1656,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1673,16 +1049,16 @@
         <v>230</v>
       </c>
       <c r="F6">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G6">
         <v>0.9</v>
       </c>
       <c r="H6">
-        <v>0.97928</v>
+        <v>0.97928000000000004</v>
       </c>
       <c r="I6">
-        <v>0.480202909076704</v>
+        <v>0.48020290907670399</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1700,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1717,16 +1093,16 @@
         <v>230</v>
       </c>
       <c r="F7">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G7">
         <v>0.9</v>
       </c>
       <c r="H7">
-        <v>0.95796</v>
+        <v>0.95796000000000003</v>
       </c>
       <c r="I7">
-        <v>0.283886529483133</v>
+        <v>0.28388652948313298</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1744,7 +1120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1761,16 +1137,16 @@
         <v>230</v>
       </c>
       <c r="F8">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G8">
         <v>0.9</v>
       </c>
       <c r="H8">
-        <v>0.9362</v>
+        <v>0.93620000000000003</v>
       </c>
       <c r="I8">
-        <v>0.126901144583254</v>
+        <v>0.12690114458325399</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1788,7 +1164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1805,16 +1181,16 @@
         <v>230</v>
       </c>
       <c r="F9">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G9">
         <v>0.9</v>
       </c>
       <c r="H9">
-        <v>0.87904</v>
+        <v>0.87904000000000004</v>
       </c>
       <c r="I9">
-        <v>-0.0805923235400888</v>
+        <v>-8.0592323540088801E-2</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1832,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1849,7 +1225,7 @@
         <v>230</v>
       </c>
       <c r="F10">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G10">
         <v>0.9</v>
@@ -1858,7 +1234,7 @@
         <v>0.89054</v>
       </c>
       <c r="I10">
-        <v>0.0936177157477223</v>
+        <v>9.3617715747722305E-2</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1876,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1893,16 +1269,16 @@
         <v>230</v>
       </c>
       <c r="F11">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G11">
         <v>0.9</v>
       </c>
       <c r="H11">
-        <v>0.82958</v>
+        <v>0.82957999999999998</v>
       </c>
       <c r="I11">
-        <v>0.336600708881117</v>
+        <v>0.33660070888111698</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1922,24 +1298,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2013,7 +1386,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2030,10 +1403,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -2075,10 +1445,10 @@
         <v>1</v>
       </c>
       <c r="U2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="V2">
-        <v>-0.3</v>
+        <v>-0.2</v>
       </c>
       <c r="W2">
         <v>1.2</v>
@@ -2089,24 +1459,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2129,7 +1496,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2154,24 +1521,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2206,7 +1570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2226,10 +1590,10 @@
         <v>11.59</v>
       </c>
       <c r="H2">
-        <v>-0.735</v>
+        <v>-0.73499999999999999</v>
       </c>
       <c r="I2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J2">
         <v>0.9</v>
@@ -2238,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2258,10 +1622,10 @@
         <v>15.75</v>
       </c>
       <c r="H3">
-        <v>-0.899</v>
+        <v>-0.89900000000000002</v>
       </c>
       <c r="I3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J3">
         <v>0.9</v>
@@ -2272,24 +1636,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2348,7 +1709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2401,7 +1762,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2454,7 +1815,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2509,24 +1870,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2588,7 +1946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2608,10 +1966,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>7.45861</v>
+        <v>7.4586100000000002</v>
       </c>
       <c r="J2">
-        <v>1.43612</v>
+        <v>1.4361200000000001</v>
       </c>
       <c r="K2">
         <v>9</v>
@@ -2641,29 +1999,26 @@
         <v>0.25</v>
       </c>
       <c r="T2">
-        <v>0.570254917162602</v>
+        <v>0.57025491716260202</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2737,7 +2092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2766,13 +2121,13 @@
         <v>230</v>
       </c>
       <c r="K2">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="L2">
         <v>0.05</v>
       </c>
       <c r="M2">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -2799,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2828,13 +2183,13 @@
         <v>230</v>
       </c>
       <c r="K3">
-        <v>0.00501</v>
+        <v>5.0099999999999997E-3</v>
       </c>
       <c r="L3">
-        <v>0.05001</v>
+        <v>5.0009999999999999E-2</v>
       </c>
       <c r="M3">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -2861,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2890,7 +2245,7 @@
         <v>230</v>
       </c>
       <c r="K4">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="L4">
         <v>0.02</v>
@@ -2923,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2952,10 +2307,10 @@
         <v>230</v>
       </c>
       <c r="K5">
-        <v>0.00201</v>
+        <v>2.0100000000000001E-3</v>
       </c>
       <c r="L5">
-        <v>0.02001</v>
+        <v>2.001E-2</v>
       </c>
       <c r="M5">
         <v>0.03</v>
@@ -2985,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3014,10 +2369,10 @@
         <v>230</v>
       </c>
       <c r="K6">
-        <v>0.02201</v>
+        <v>2.2009999999999998E-2</v>
       </c>
       <c r="L6">
-        <v>0.22001</v>
+        <v>0.22001000000000001</v>
       </c>
       <c r="M6">
         <v>0.33</v>
@@ -3047,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3076,10 +2431,10 @@
         <v>230</v>
       </c>
       <c r="K7">
-        <v>0.02202</v>
+        <v>2.2020000000000001E-2</v>
       </c>
       <c r="L7">
-        <v>0.22002</v>
+        <v>0.22001999999999999</v>
       </c>
       <c r="M7">
         <v>0.33</v>
@@ -3109,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3138,7 +2493,7 @@
         <v>230</v>
       </c>
       <c r="K8">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="L8">
         <v>0.22</v>
@@ -3171,7 +2526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3200,7 +2555,7 @@
         <v>230</v>
       </c>
       <c r="K9">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="L9">
         <v>0.02</v>
@@ -3233,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3262,10 +2617,10 @@
         <v>230</v>
       </c>
       <c r="K10">
-        <v>0.00201</v>
+        <v>2.0100000000000001E-3</v>
       </c>
       <c r="L10">
-        <v>0.02001</v>
+        <v>2.001E-2</v>
       </c>
       <c r="M10">
         <v>0.03</v>
@@ -3295,7 +2650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3324,13 +2679,13 @@
         <v>230</v>
       </c>
       <c r="K11">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="L11">
         <v>0.05</v>
       </c>
       <c r="M11">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -3357,7 +2712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3386,13 +2741,13 @@
         <v>230</v>
       </c>
       <c r="K12">
-        <v>0.00501</v>
+        <v>5.0099999999999997E-3</v>
       </c>
       <c r="L12">
-        <v>0.05001</v>
+        <v>5.0009999999999999E-2</v>
       </c>
       <c r="M12">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -3419,7 +2774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3448,10 +2803,10 @@
         <v>230</v>
       </c>
       <c r="K13">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L13">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -3481,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3510,10 +2865,10 @@
         <v>230</v>
       </c>
       <c r="K14">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L14">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -3543,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3572,10 +2927,10 @@
         <v>230</v>
       </c>
       <c r="K15">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L15">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -3605,7 +2960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3634,10 +2989,10 @@
         <v>230</v>
       </c>
       <c r="K16">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="L16">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -3669,24 +3024,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3700,7 +3052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3714,7 +3066,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3730,24 +3082,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3833,7 +3182,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3898,7 +3247,7 @@
         <v>0.25</v>
       </c>
       <c r="W2">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X2">
         <v>0.25</v>
@@ -3916,7 +3265,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3981,7 +3330,7 @@
         <v>0.25</v>
       </c>
       <c r="W3">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X3">
         <v>0.25</v>
@@ -3999,7 +3348,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4064,7 +3413,7 @@
         <v>0.25</v>
       </c>
       <c r="W4">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X4">
         <v>0.25</v>
@@ -4082,7 +3431,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4147,7 +3496,7 @@
         <v>0.25</v>
       </c>
       <c r="W5">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X5">
         <v>0.25</v>
@@ -4167,24 +3516,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4225,7 +3571,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4266,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4307,7 +3653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4348,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4391,24 +3737,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4476,7 +3819,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4511,7 +3854,7 @@
         <v>1.246</v>
       </c>
       <c r="L2">
-        <v>0.0754</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M2">
         <v>20</v>
@@ -4544,7 +3887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4579,7 +3922,7 @@
         <v>1.246</v>
       </c>
       <c r="L3">
-        <v>0.0754</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M3">
         <v>20</v>
@@ -4612,7 +3955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4647,7 +3990,7 @@
         <v>1.246</v>
       </c>
       <c r="L4">
-        <v>0.0754</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M4">
         <v>20</v>
@@ -4680,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4715,7 +4058,7 @@
         <v>1.246</v>
       </c>
       <c r="L5">
-        <v>0.0754</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="M5">
         <v>20</v>
@@ -4750,6 +4093,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>